<commit_message>
collate soil nutrient data and start merging soil data, phys data, and multispeq data into single dataset
</commit_message>
<xml_diff>
--- a/licor_data/licor_log_files/licor_log_file_blank.xlsx
+++ b/licor_data/licor_log_files/licor_log_file_blank.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11210"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eaperkowski/git/trillium_trail/licor_data/licor_log_files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eaperkowski/git/2023_TT_phys/licor_data/licor_log_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09DD0CAD-A91C-0442-962D-DCA4D7E3CAEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4773412C-44FC-2D41-B7F0-14D0ECA89490}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1660" yWindow="500" windowWidth="28800" windowHeight="15620" xr2:uid="{E2101264-4A8C-BA4C-A9EF-E5EFE562CDE8}"/>
+    <workbookView xWindow="1720" yWindow="500" windowWidth="28800" windowHeight="28260" xr2:uid="{E2101264-4A8C-BA4C-A9EF-E5EFE562CDE8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="18">
   <si>
     <t>LICOR CHAMBER CONDITIONS</t>
   </si>
@@ -90,26 +90,14 @@
     <t>TEMP (Tleaf, degC):</t>
   </si>
   <si>
-    <t>Tleaf = 25</t>
-  </si>
-  <si>
-    <t>420 (before curve)</t>
-  </si>
-  <si>
-    <t>MAI</t>
-  </si>
-  <si>
-    <t>NO TIME</t>
-  </si>
-  <si>
-    <t>STARTED TOO SOON; MAY BE BAD CURVE</t>
+    <t>_________</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -152,13 +140,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="15"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -195,7 +176,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -212,14 +193,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -540,7 +518,7 @@
   <dimension ref="A1:H26"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="86" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -578,12 +556,8 @@
       </c>
     </row>
     <row r="2" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A2" s="6">
-        <v>2616</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>19</v>
-      </c>
+      <c r="A2" s="6"/>
+      <c r="B2" s="6"/>
       <c r="C2" s="5" t="s">
         <v>5</v>
       </c>
@@ -596,18 +570,12 @@
       <c r="F2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="11">
-        <v>0.46527777777777773</v>
-      </c>
+      <c r="G2" s="8"/>
       <c r="H2" s="7"/>
     </row>
     <row r="3" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A3" s="6">
-        <v>1476</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>19</v>
-      </c>
+      <c r="A3" s="6"/>
+      <c r="B3" s="6"/>
       <c r="C3" s="5" t="s">
         <v>5</v>
       </c>
@@ -620,18 +588,12 @@
       <c r="F3" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="11">
-        <v>0.52500000000000002</v>
-      </c>
+      <c r="G3" s="8"/>
       <c r="H3" s="7"/>
     </row>
     <row r="4" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A4" s="6">
-        <v>4781</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>19</v>
-      </c>
+      <c r="A4" s="6"/>
+      <c r="B4" s="6"/>
       <c r="C4" s="5" t="s">
         <v>5</v>
       </c>
@@ -644,20 +606,12 @@
       <c r="F4" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G4" s="11">
-        <v>0.53749999999999998</v>
-      </c>
-      <c r="H4" s="7" t="s">
-        <v>21</v>
-      </c>
+      <c r="G4" s="8"/>
+      <c r="H4" s="7"/>
     </row>
     <row r="5" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A5" s="6">
-        <v>5052</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>19</v>
-      </c>
+      <c r="A5" s="6"/>
+      <c r="B5" s="6"/>
       <c r="C5" s="5" t="s">
         <v>5</v>
       </c>
@@ -670,9 +624,7 @@
       <c r="F5" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G5" s="7" t="s">
-        <v>20</v>
-      </c>
+      <c r="G5" s="7"/>
       <c r="H5" s="7"/>
     </row>
     <row r="6" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.45">
@@ -938,15 +890,15 @@
         <v>1</v>
       </c>
       <c r="B22" s="9"/>
-      <c r="C22" s="4">
-        <v>500</v>
+      <c r="C22" s="4" t="s">
+        <v>17</v>
       </c>
       <c r="E22" s="9" t="s">
         <v>4</v>
       </c>
       <c r="F22" s="9"/>
-      <c r="G22" s="4">
-        <v>10000</v>
+      <c r="G22" s="4" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.3">
@@ -954,8 +906,8 @@
         <v>2</v>
       </c>
       <c r="B23" s="9"/>
-      <c r="C23" s="4">
-        <v>1.5</v>
+      <c r="C23" s="4" t="s">
+        <v>17</v>
       </c>
       <c r="E23" s="10" t="s">
         <v>16</v>
@@ -970,15 +922,15 @@
         <v>3</v>
       </c>
       <c r="B24" s="9"/>
-      <c r="C24" s="8" t="s">
-        <v>18</v>
+      <c r="C24" s="4" t="s">
+        <v>17</v>
       </c>
       <c r="E24" s="10" t="s">
         <v>6</v>
       </c>
       <c r="F24" s="10"/>
-      <c r="G24" s="4">
-        <v>1600</v>
+      <c r="G24" s="4" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="26" x14ac:dyDescent="0.3">
@@ -1006,12 +958,12 @@
     <mergeCell ref="E24:F24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="48" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="50"/>
+  <pageSetup scale="48" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="20"/>
   <headerFooter alignWithMargins="0">
-    <oddHeader>&amp;L&amp;"Calibri (Body),Regular"&amp;24
-Date: JUNE 15, 2023&amp;C&amp;"Calibri (Body),Regular"&amp;18Machine (circle):
-&amp;24Ozz   Gib    Alb    Stan    &amp;"Calibri (Body),Bold"Yat&amp;R&amp;"Calibri (Body),Regular"&amp;20
-Licor Enthusiast: EVAN PERKOWSKI</oddHeader>
+    <oddHeader xml:space="preserve">&amp;L&amp;"Calibri (Body),Regular"&amp;24
+Date:&amp;C&amp;"Calibri (Body),Regular"&amp;18Machine (circle):
+&amp;24Ozz   Gib    Alb    Stan&amp;"-,Regular"&amp;30    &amp;"Calibri (Body),Regular"&amp;24Yat&amp;R&amp;"Calibri (Body),Regular"&amp;20
+Licor Enthusiast: ___________________   </oddHeader>
     <oddFooter>&amp;L&amp;"Calibri (Body),Regular"&amp;20Weather notes:</oddFooter>
   </headerFooter>
 </worksheet>

</xml_diff>